<commit_message>
feat: update article line ranges
</commit_message>
<xml_diff>
--- a/docs/articles_metadata.xlsx
+++ b/docs/articles_metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/github/modelling-marti/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736B632F-1A64-114A-B202-7F6F7A6E1A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81CA4D-7CCD-F844-8EB7-710BB00C8039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{01E6211F-D14A-5F4F-930C-D0490E6F2E5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE9704E-F4DE-0E4D-894D-7A1738F79AC1}">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2779,10 +2779,10 @@
         <v>385</v>
       </c>
       <c r="G59">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H59">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2831,10 +2831,10 @@
         <v>385</v>
       </c>
       <c r="G61">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H61">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2909,10 +2909,10 @@
         <v>385</v>
       </c>
       <c r="G64">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H64">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2935,10 +2935,10 @@
         <v>386</v>
       </c>
       <c r="G65">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H65">
-        <v>728</v>
+        <v>720</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2961,10 +2961,10 @@
         <v>386</v>
       </c>
       <c r="G66">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H66">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2987,10 +2987,10 @@
         <v>385</v>
       </c>
       <c r="G67">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H67">
-        <v>271</v>
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -3013,10 +3013,10 @@
         <v>385</v>
       </c>
       <c r="G68">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="H68">
-        <v>944</v>
+        <v>924</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -3039,10 +3039,10 @@
         <v>385</v>
       </c>
       <c r="G69">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H69">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -3065,10 +3065,10 @@
         <v>385</v>
       </c>
       <c r="G70">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H70">
-        <v>2582</v>
+        <v>2574</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -3091,10 +3091,10 @@
         <v>385</v>
       </c>
       <c r="G71">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H71">
-        <v>1171</v>
+        <v>937</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -3117,10 +3117,10 @@
         <v>385</v>
       </c>
       <c r="G72">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H72">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -3143,10 +3143,10 @@
         <v>385</v>
       </c>
       <c r="G73">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H73">
-        <v>379</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -3169,10 +3169,10 @@
         <v>385</v>
       </c>
       <c r="G74">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H74">
-        <v>863</v>
+        <v>856</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -3195,10 +3195,10 @@
         <v>385</v>
       </c>
       <c r="G75">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H75">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -3221,10 +3221,10 @@
         <v>385</v>
       </c>
       <c r="G76">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H76">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -3247,10 +3247,10 @@
         <v>385</v>
       </c>
       <c r="G77">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H77">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -3273,10 +3273,10 @@
         <v>385</v>
       </c>
       <c r="G78">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H78">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -3299,10 +3299,10 @@
         <v>385</v>
       </c>
       <c r="G79">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H79">
-        <v>997</v>
+        <v>990</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -3325,10 +3325,10 @@
         <v>385</v>
       </c>
       <c r="G80">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H80">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -3351,10 +3351,10 @@
         <v>385</v>
       </c>
       <c r="G81">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H81">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -3377,10 +3377,10 @@
         <v>385</v>
       </c>
       <c r="G82">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H82">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -3403,10 +3403,10 @@
         <v>385</v>
       </c>
       <c r="G83">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H83">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -3429,10 +3429,10 @@
         <v>385</v>
       </c>
       <c r="G84">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H84">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -3455,10 +3455,10 @@
         <v>385</v>
       </c>
       <c r="G85">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="H85">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -3481,10 +3481,10 @@
         <v>385</v>
       </c>
       <c r="G86">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H86">
-        <v>635</v>
+        <v>627</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -3507,10 +3507,10 @@
         <v>385</v>
       </c>
       <c r="G87">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="H87">
-        <v>859</v>
+        <v>839</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -3533,10 +3533,10 @@
         <v>385</v>
       </c>
       <c r="G88">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H88">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -3559,10 +3559,10 @@
         <v>385</v>
       </c>
       <c r="G89">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="H89">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -3585,10 +3585,10 @@
         <v>385</v>
       </c>
       <c r="G90">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="H90">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -3611,10 +3611,10 @@
         <v>385</v>
       </c>
       <c r="G91">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="H91">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -3637,10 +3637,10 @@
         <v>385</v>
       </c>
       <c r="G92">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="H92">
-        <v>987</v>
+        <v>968</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -3663,10 +3663,10 @@
         <v>386</v>
       </c>
       <c r="G93">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H93">
-        <v>795</v>
+        <v>788</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -3689,10 +3689,10 @@
         <v>386</v>
       </c>
       <c r="G94">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H94">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -3715,10 +3715,10 @@
         <v>385</v>
       </c>
       <c r="G95">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H95">
-        <v>597</v>
+        <v>591</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -3741,10 +3741,10 @@
         <v>385</v>
       </c>
       <c r="G96">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="H96">
-        <v>891</v>
+        <v>883</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -3767,10 +3767,10 @@
         <v>385</v>
       </c>
       <c r="G97">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H97">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3793,10 +3793,10 @@
         <v>385</v>
       </c>
       <c r="G98">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H98">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3819,10 +3819,10 @@
         <v>385</v>
       </c>
       <c r="G99">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="H99">
-        <v>532</v>
+        <v>513</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -3845,10 +3845,10 @@
         <v>385</v>
       </c>
       <c r="G100">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="H100">
-        <v>601</v>
+        <v>582</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
@@ -3871,10 +3871,10 @@
         <v>385</v>
       </c>
       <c r="G101">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H101">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
@@ -3897,10 +3897,10 @@
         <v>385</v>
       </c>
       <c r="G102">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H102">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
@@ -3923,10 +3923,10 @@
         <v>385</v>
       </c>
       <c r="G103">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H103">
-        <v>890</v>
+        <v>883</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3949,10 +3949,10 @@
         <v>385</v>
       </c>
       <c r="G104">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="H104">
-        <v>594</v>
+        <v>575</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3975,10 +3975,10 @@
         <v>385</v>
       </c>
       <c r="G105">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H105">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -4001,10 +4001,10 @@
         <v>385</v>
       </c>
       <c r="G106">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H106">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -4027,10 +4027,10 @@
         <v>385</v>
       </c>
       <c r="G107">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="H107">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -4053,10 +4053,10 @@
         <v>385</v>
       </c>
       <c r="G108">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="H108">
-        <v>393</v>
+        <v>374</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -4079,10 +4079,10 @@
         <v>385</v>
       </c>
       <c r="G109">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H109">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -4105,10 +4105,10 @@
         <v>385</v>
       </c>
       <c r="G110">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H110">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -4131,10 +4131,10 @@
         <v>385</v>
       </c>
       <c r="G111">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H111">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -4157,10 +4157,10 @@
         <v>385</v>
       </c>
       <c r="G112">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H112">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -4183,10 +4183,10 @@
         <v>385</v>
       </c>
       <c r="G113">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -4209,10 +4209,10 @@
         <v>385</v>
       </c>
       <c r="G114">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="H114">
-        <v>755</v>
+        <v>748</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -4235,10 +4235,10 @@
         <v>385</v>
       </c>
       <c r="G115">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H115">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -4261,10 +4261,10 @@
         <v>385</v>
       </c>
       <c r="G116">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H116">
-        <v>766</v>
+        <v>760</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -4287,10 +4287,10 @@
         <v>385</v>
       </c>
       <c r="G117">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H117">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -4313,10 +4313,10 @@
         <v>385</v>
       </c>
       <c r="G118">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H118">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -4339,10 +4339,10 @@
         <v>385</v>
       </c>
       <c r="G119">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H119">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -4365,10 +4365,10 @@
         <v>385</v>
       </c>
       <c r="G120">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H120">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -4391,10 +4391,10 @@
         <v>385</v>
       </c>
       <c r="G121">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H121">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -4417,10 +4417,10 @@
         <v>385</v>
       </c>
       <c r="G122">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H122">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -4443,10 +4443,10 @@
         <v>385</v>
       </c>
       <c r="G123">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="H123">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -4469,10 +4469,10 @@
         <v>385</v>
       </c>
       <c r="G124">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H124">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -4495,10 +4495,10 @@
         <v>385</v>
       </c>
       <c r="G125">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="H125">
-        <v>300</v>
+        <v>294</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -4521,10 +4521,10 @@
         <v>385</v>
       </c>
       <c r="G126">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="H126">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -4547,10 +4547,10 @@
         <v>385</v>
       </c>
       <c r="G127">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H127">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -4573,10 +4573,10 @@
         <v>385</v>
       </c>
       <c r="G128">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H128">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -4599,10 +4599,10 @@
         <v>385</v>
       </c>
       <c r="G129">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H129">
-        <v>879</v>
+        <v>873</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -4625,10 +4625,10 @@
         <v>385</v>
       </c>
       <c r="G130">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H130">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -4651,10 +4651,10 @@
         <v>385</v>
       </c>
       <c r="G131">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H131">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
@@ -4677,10 +4677,10 @@
         <v>385</v>
       </c>
       <c r="G132">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H132">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -4703,10 +4703,10 @@
         <v>385</v>
       </c>
       <c r="G133">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H133">
-        <v>519</v>
+        <v>513</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -4729,10 +4729,10 @@
         <v>385</v>
       </c>
       <c r="G134">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H134">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
@@ -4755,10 +4755,10 @@
         <v>386</v>
       </c>
       <c r="G135">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H135">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4781,10 +4781,10 @@
         <v>386</v>
       </c>
       <c r="G136">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H136">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4807,10 +4807,10 @@
         <v>386</v>
       </c>
       <c r="G137">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H137">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -4833,10 +4833,10 @@
         <v>385</v>
       </c>
       <c r="G138">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H138">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -4859,10 +4859,10 @@
         <v>385</v>
       </c>
       <c r="G139">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H139">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -4885,10 +4885,10 @@
         <v>385</v>
       </c>
       <c r="G140">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H140">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4911,10 +4911,10 @@
         <v>385</v>
       </c>
       <c r="G141">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H141">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4937,10 +4937,10 @@
         <v>386</v>
       </c>
       <c r="G142">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H142">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4963,10 +4963,10 @@
         <v>386</v>
       </c>
       <c r="G143">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H143">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4989,10 +4989,10 @@
         <v>385</v>
       </c>
       <c r="G144">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H144">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -5015,10 +5015,10 @@
         <v>385</v>
       </c>
       <c r="G145">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H145">
-        <v>566</v>
+        <v>560</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -5041,10 +5041,10 @@
         <v>385</v>
       </c>
       <c r="G146">
-        <v>1003</v>
+        <v>995</v>
       </c>
       <c r="H146">
-        <v>1027</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -5067,10 +5067,10 @@
         <v>385</v>
       </c>
       <c r="G147">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H147">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -5093,10 +5093,10 @@
         <v>385</v>
       </c>
       <c r="G148">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H148">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -5119,10 +5119,10 @@
         <v>385</v>
       </c>
       <c r="G149">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="H149">
-        <v>851</v>
+        <v>844</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -5145,10 +5145,10 @@
         <v>385</v>
       </c>
       <c r="G150">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H150">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -5171,10 +5171,10 @@
         <v>385</v>
       </c>
       <c r="G151">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H151">
-        <v>708</v>
+        <v>702</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -5197,10 +5197,10 @@
         <v>385</v>
       </c>
       <c r="G152">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H152">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -5223,10 +5223,10 @@
         <v>385</v>
       </c>
       <c r="G153">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H153">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -5249,10 +5249,10 @@
         <v>385</v>
       </c>
       <c r="G154">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H154">
-        <v>1020</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -5275,10 +5275,10 @@
         <v>385</v>
       </c>
       <c r="G155">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H155">
-        <v>340</v>
+        <v>321</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -5301,10 +5301,10 @@
         <v>386</v>
       </c>
       <c r="G156">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H156">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -5327,10 +5327,10 @@
         <v>386</v>
       </c>
       <c r="G157">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H157">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -5353,10 +5353,10 @@
         <v>385</v>
       </c>
       <c r="G158">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H158">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -5379,10 +5379,10 @@
         <v>385</v>
       </c>
       <c r="G159">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H159">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -5405,10 +5405,10 @@
         <v>385</v>
       </c>
       <c r="G160">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H160">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -5431,10 +5431,10 @@
         <v>385</v>
       </c>
       <c r="G161">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H161">
-        <v>912</v>
+        <v>906</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
@@ -5457,10 +5457,10 @@
         <v>385</v>
       </c>
       <c r="G162">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H162">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -5483,10 +5483,10 @@
         <v>385</v>
       </c>
       <c r="G163">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H163">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -5509,10 +5509,10 @@
         <v>385</v>
       </c>
       <c r="G164">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H164">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -5535,10 +5535,10 @@
         <v>385</v>
       </c>
       <c r="G165">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H165">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
@@ -5561,10 +5561,10 @@
         <v>385</v>
       </c>
       <c r="G166">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H166">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -5587,10 +5587,10 @@
         <v>385</v>
       </c>
       <c r="G167">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H167">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -5613,10 +5613,10 @@
         <v>385</v>
       </c>
       <c r="G168">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H168">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -5639,10 +5639,10 @@
         <v>385</v>
       </c>
       <c r="G169">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H169">
-        <v>580</v>
+        <v>572</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -5665,10 +5665,10 @@
         <v>386</v>
       </c>
       <c r="G170">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H170">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -5691,10 +5691,10 @@
         <v>386</v>
       </c>
       <c r="G171">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H171">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -5717,10 +5717,10 @@
         <v>385</v>
       </c>
       <c r="G172">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H172">
-        <v>750</v>
+        <v>744</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -5743,10 +5743,10 @@
         <v>385</v>
       </c>
       <c r="G173">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H173">
-        <v>1164</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -5769,10 +5769,10 @@
         <v>385</v>
       </c>
       <c r="G174">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H174">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -5795,10 +5795,10 @@
         <v>385</v>
       </c>
       <c r="G175">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H175">
-        <v>840</v>
+        <v>833</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -5821,10 +5821,10 @@
         <v>385</v>
       </c>
       <c r="G176">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H176">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -5847,10 +5847,10 @@
         <v>385</v>
       </c>
       <c r="G177">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H177">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -5873,10 +5873,10 @@
         <v>385</v>
       </c>
       <c r="G178">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H178">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -5899,10 +5899,10 @@
         <v>385</v>
       </c>
       <c r="G179">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H179">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -5925,10 +5925,10 @@
         <v>385</v>
       </c>
       <c r="G180">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H180">
-        <v>416</v>
+        <v>410</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -5951,10 +5951,10 @@
         <v>385</v>
       </c>
       <c r="G181">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H181">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -5977,10 +5977,10 @@
         <v>385</v>
       </c>
       <c r="G182">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H182">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -6003,10 +6003,10 @@
         <v>385</v>
       </c>
       <c r="G183">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="H183">
-        <v>494</v>
+        <v>487</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -6029,10 +6029,10 @@
         <v>385</v>
       </c>
       <c r="G184">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H184">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -6055,10 +6055,10 @@
         <v>385</v>
       </c>
       <c r="G185">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H185">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -6081,10 +6081,10 @@
         <v>385</v>
       </c>
       <c r="G186">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H186">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -6107,10 +6107,10 @@
         <v>385</v>
       </c>
       <c r="G187">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H187">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -6133,10 +6133,10 @@
         <v>386</v>
       </c>
       <c r="G188">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H188">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -6159,10 +6159,10 @@
         <v>386</v>
       </c>
       <c r="G189">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H189">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: correct article boundary lines
</commit_message>
<xml_diff>
--- a/docs/articles_metadata.xlsx
+++ b/docs/articles_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/github/modelling-marti/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81CA4D-7CCD-F844-8EB7-710BB00C8039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E2B84-9F38-1143-9FDF-8549123B56CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{01E6211F-D14A-5F4F-930C-D0490E6F2E5E}"/>
   </bookViews>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE9704E-F4DE-0E4D-894D-7A1738F79AC1}">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3117,10 +3117,10 @@
         <v>385</v>
       </c>
       <c r="G72">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H72">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -3143,7 +3143,7 @@
         <v>385</v>
       </c>
       <c r="G73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H73">
         <v>370</v>
@@ -3744,7 +3744,7 @@
         <v>113</v>
       </c>
       <c r="H96">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -4469,10 +4469,10 @@
         <v>385</v>
       </c>
       <c r="G124">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H124">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -5795,10 +5795,10 @@
         <v>385</v>
       </c>
       <c r="G175">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H175">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: improve article boundaries for ror-002_1971_50__512_d
</commit_message>
<xml_diff>
--- a/docs/articles_metadata.xlsx
+++ b/docs/articles_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/github/modelling-marti/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E2B84-9F38-1143-9FDF-8549123B56CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2095A5E-60D4-F545-9912-254C1BDBD857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{01E6211F-D14A-5F4F-930C-D0490E6F2E5E}"/>
   </bookViews>
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE9704E-F4DE-0E4D-894D-7A1738F79AC1}">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3377,7 +3377,7 @@
         <v>385</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="H82">
         <v>602</v>

</xml_diff>

<commit_message>
feat: add NZZ article line boundaries
</commit_message>
<xml_diff>
--- a/docs/articles_metadata.xlsx
+++ b/docs/articles_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtwente/github/modelling-marti/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2095A5E-60D4-F545-9912-254C1BDBD857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E23DC0-84BF-FE48-820B-2D83FF85F20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{01E6211F-D14A-5F4F-930C-D0490E6F2E5E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="390">
   <si>
     <t>id</t>
   </si>
@@ -1203,6 +1203,9 @@
   </si>
   <si>
     <t>last_row</t>
+  </si>
+  <si>
+    <t>xxx falsch, vertauscht?</t>
   </si>
 </sst>
 </file>
@@ -1575,10 +1578,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE9704E-F4DE-0E4D-894D-7A1738F79AC1}">
-  <dimension ref="A1:H189"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1638,6 +1642,12 @@
       <c r="F2" t="s">
         <v>385</v>
       </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1658,6 +1668,12 @@
       <c r="F3" t="s">
         <v>385</v>
       </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1678,6 +1694,12 @@
       <c r="F4" t="s">
         <v>385</v>
       </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1698,6 +1720,12 @@
       <c r="F5" t="s">
         <v>385</v>
       </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1718,6 +1746,12 @@
       <c r="F6" t="s">
         <v>385</v>
       </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1738,6 +1772,12 @@
       <c r="F7" t="s">
         <v>385</v>
       </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1758,6 +1798,12 @@
       <c r="F8" t="s">
         <v>386</v>
       </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1778,6 +1824,12 @@
       <c r="F9" t="s">
         <v>386</v>
       </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1798,6 +1850,12 @@
       <c r="F10" t="s">
         <v>385</v>
       </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1818,6 +1876,12 @@
       <c r="F11" t="s">
         <v>385</v>
       </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1838,6 +1902,12 @@
       <c r="F12" t="s">
         <v>385</v>
       </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1858,6 +1928,12 @@
       <c r="F13" t="s">
         <v>385</v>
       </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1878,6 +1954,12 @@
       <c r="F14" t="s">
         <v>385</v>
       </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1898,6 +1980,12 @@
       <c r="F15" t="s">
         <v>385</v>
       </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1918,8 +2006,14 @@
       <c r="F16" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1938,8 +2032,14 @@
       <c r="F17" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1958,8 +2058,14 @@
       <c r="F18" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1978,8 +2084,14 @@
       <c r="F19" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1998,8 +2110,14 @@
       <c r="F20" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2018,8 +2136,14 @@
       <c r="F21" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2038,8 +2162,14 @@
       <c r="F22" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2058,8 +2188,14 @@
       <c r="F23" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2078,8 +2214,14 @@
       <c r="F24" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2098,8 +2240,14 @@
       <c r="F25" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2118,8 +2266,14 @@
       <c r="F26" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2138,8 +2292,14 @@
       <c r="F27" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2158,8 +2318,14 @@
       <c r="F28" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2178,8 +2344,14 @@
       <c r="F29" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2198,8 +2370,14 @@
       <c r="F30" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2218,8 +2396,14 @@
       <c r="F31" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2238,8 +2422,14 @@
       <c r="F32" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2258,8 +2448,14 @@
       <c r="F33" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2278,8 +2474,14 @@
       <c r="F34" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2298,8 +2500,14 @@
       <c r="F35" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2318,8 +2526,14 @@
       <c r="F36" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2338,8 +2552,14 @@
       <c r="F37" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2358,8 +2578,14 @@
       <c r="F38" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2378,8 +2604,14 @@
       <c r="F39" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2398,8 +2630,14 @@
       <c r="F40" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2418,8 +2656,14 @@
       <c r="F41" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2438,8 +2682,14 @@
       <c r="F42" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2458,8 +2708,14 @@
       <c r="F43" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2478,8 +2734,14 @@
       <c r="F44" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2498,8 +2760,14 @@
       <c r="F45" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -2518,8 +2786,14 @@
       <c r="F46" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2538,8 +2812,17 @@
       <c r="F47" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -2557,6 +2840,12 @@
       </c>
       <c r="F48" t="s">
         <v>386</v>
+      </c>
+      <c r="G48">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2578,6 +2867,12 @@
       <c r="F49" t="s">
         <v>386</v>
       </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -2598,6 +2893,12 @@
       <c r="F50" t="s">
         <v>386</v>
       </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -2618,6 +2919,12 @@
       <c r="F51" t="s">
         <v>385</v>
       </c>
+      <c r="G51">
+        <v>3</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2638,6 +2945,12 @@
       <c r="F52" t="s">
         <v>385</v>
       </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -2658,6 +2971,12 @@
       <c r="F53" t="s">
         <v>385</v>
       </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -2678,6 +2997,12 @@
       <c r="F54" t="s">
         <v>385</v>
       </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>26</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -2698,6 +3023,12 @@
       <c r="F55" t="s">
         <v>385</v>
       </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -2718,6 +3049,12 @@
       <c r="F56" t="s">
         <v>385</v>
       </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>6</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -2738,6 +3075,12 @@
       <c r="F57" t="s">
         <v>385</v>
       </c>
+      <c r="G57">
+        <v>4</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -2757,6 +3100,12 @@
       </c>
       <c r="F58" t="s">
         <v>385</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>